<commit_message>
Added Initial Design Concept Document under documentation [Nick]
</commit_message>
<xml_diff>
--- a/documentation/initial_burndown_chart.xlsx
+++ b/documentation/initial_burndown_chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholascashiola/Documents/CSCE315/csce_315_hci_project/CSCE-315-Project-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2115226B-9314-4141-A725-AAABA5F107B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8399FC5-BFBA-4C44-954D-D818FD45C350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{9A23A667-1736-F64E-BFE7-7EF1FE99DA74}"/>
   </bookViews>
@@ -135,6 +135,1131 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Initial Burndown Chart (pre-Sprint 1)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE5F-E441-B639-A3719489F8CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1566493344"/>
+        <c:axId val="1565840944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1566493344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days Left</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1565840944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1565840944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1566493344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BBE8B2F-1A8D-0C49-AB42-C422D5A56098}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,7 +1562,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +1594,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3">
         <v>50</v>
@@ -477,7 +1602,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>40</v>
@@ -485,7 +1610,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>30</v>
@@ -493,7 +1618,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>20</v>
@@ -501,7 +1626,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>10</v>
@@ -509,7 +1634,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -517,5 +1642,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed burndown chart [Nick]
</commit_message>
<xml_diff>
--- a/documentation/initial_burndown_chart.xlsx
+++ b/documentation/initial_burndown_chart.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholascashiola/Documents/CSCE315/csce_315_hci_project/CSCE-315-Project-2/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8399FC5-BFBA-4C44-954D-D818FD45C350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DEB207-80F6-A344-96A3-B662E49956E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{9A23A667-1736-F64E-BFE7-7EF1FE99DA74}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{9A23A667-1736-F64E-BFE7-7EF1FE99DA74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3:$B$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3:$C$9</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$3:$B$9</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$C$3:$C$9</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -171,11 +177,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Initial Burndown Chart (pre-Sprint 1)</a:t>
+              <a:t>Initial Burndown Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32338188976377952"/>
+          <c:y val="3.7037037037037035E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -207,8 +221,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -229,65 +243,59 @@
             </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$9</c:f>
               <c:numCache>
@@ -316,29 +324,27 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CE5F-E441-B639-A3719489F8CC}"/>
+              <c16:uniqueId val="{00000000-92F6-774C-AFAB-4C916B729E5B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1566493344"/>
-        <c:axId val="1565840944"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1566493344"/>
+        <c:axId val="1568332624"/>
+        <c:axId val="1568528080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1568332624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,23 +353,13 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -422,6 +418,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -451,15 +448,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1565840944"/>
+        <c:crossAx val="1568528080"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1565840944"/>
+        <c:axId val="1568528080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,23 +462,13 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -510,7 +494,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Tasks Remaining</a:t>
+                  <a:t>Task Remaining</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -549,8 +533,13 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -573,9 +562,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1566493344"/>
+        <c:crossAx val="1568332624"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -587,13 +576,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -673,7 +655,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -873,7 +855,7 @@
       </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -986,27 +968,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -1016,29 +988,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -1208,7 +1168,18 @@
         <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1231,17 +1202,17 @@
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BBE8B2F-1A8D-0C49-AB42-C422D5A56098}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF19A56-1297-7D49-A374-9C6DA5FDCEEF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,7 +1533,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>